<commit_message>
Changes to TC003_LoginDDT and changing to testname give dynamically and unique
</commit_message>
<xml_diff>
--- a/testData/OpenCart_LoginData.xlsx
+++ b/testData/OpenCart_LoginData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>test12345</t>
+  </si>
+  <si>
+    <t>bhaskar4@gmail.com</t>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>bhaskar3@gmail.com</t>
+  </si>
+  <si>
+    <t>Test12345</t>
   </si>
 </sst>
 </file>
@@ -78,7 +90,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,13 +112,6 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -564,157 +569,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,7 +729,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1061,13 +1067,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="36.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1128,9 +1134,33 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="bhaskar@gmail.com"/>
+    <hyperlink ref="A6" r:id="rId2" display="bhaskar4@gmail.com" tooltip="mailto:bhaskar4@gmail.com"/>
+    <hyperlink ref="A7" r:id="rId3" display="bhaskar3@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>